<commit_message>
Fix success rate precision
</commit_message>
<xml_diff>
--- a/info/Min-max/Alpha Analysis.xlsx
+++ b/info/Min-max/Alpha Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5604" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5604" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Alpha Analysis" sheetId="2" r:id="rId1"/>
@@ -225,21 +225,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW" i="1"/>
-              <a:t>α </a:t>
+              <a:rPr lang="en-US" altLang="zh-TW" b="1" i="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Overall</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>/ </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" i="1"/>
-              <a:t>NP</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="800"/>
-              <a:t>2</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US" sz="800" b="1" i="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -303,7 +300,7 @@
                 <a:schemeClr val="bg1"/>
               </a:bgClr>
             </a:pattFill>
-            <a:ln w="9525">
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -326,10 +323,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -416,25 +410,25 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.8522222222222221E-2</c:v>
+                  <c:v>1.7777777777777778E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63888888888888884</c:v>
+                  <c:v>0.63777777777777778</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79628888888888882</c:v>
+                  <c:v>0.79555555555555557</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96296666666666653</c:v>
+                  <c:v>0.9622222222222222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93518888888888896</c:v>
+                  <c:v>0.93555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96296666666666653</c:v>
+                  <c:v>0.9622222222222222</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96759259259259245</c:v>
+                  <c:v>0.96666666666666656</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.97333333333333327</c:v>
@@ -443,10 +437,10 @@
                   <c:v>0.97333333333333327</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.93981481481481488</c:v>
+                  <c:v>0.94000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.87963333333333327</c:v>
+                  <c:v>0.87777777777777777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -460,19 +454,100 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="100"/>
         <c:overlap val="-27"/>
-        <c:axId val="204821376"/>
-        <c:axId val="204999312"/>
+        <c:axId val="205251344"/>
+        <c:axId val="205251904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="204821376"/>
+        <c:axId val="205251344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Propagation Ratio (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" b="1" i="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>α%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -480,9 +555,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -496,10 +570,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -509,7 +580,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204999312"/>
+        <c:crossAx val="205251904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -517,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204999312"/>
+        <c:axId val="205251904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -528,9 +599,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -538,6 +608,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Success Rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -556,10 +691,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -569,14 +701,18 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204821376"/>
+        <c:crossAx val="205251344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1461,7 +1597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1535,11 +1673,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>0.16669999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="K2" s="5">
         <f>AVERAGE(B2:J2)</f>
-        <v>1.8522222222222221E-2</v>
+        <v>1.7777777777777778E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1571,11 +1709,11 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3:K12" si="0">AVERAGE(B3:J3)</f>
-        <v>0.63888888888888884</v>
+        <v>0.63777777777777778</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1595,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>8.3299999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -1604,14 +1742,14 @@
         <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>0.58330000000000004</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="0"/>
-        <v>0.79628888888888882</v>
+        <v>0.79555555555555557</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1631,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -1647,7 +1785,7 @@
       </c>
       <c r="K5" s="5">
         <f t="shared" si="0"/>
-        <v>0.96296666666666653</v>
+        <v>0.9622222222222222</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1658,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>0.91669999999999996</v>
+        <v>0.92</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1683,7 +1821,7 @@
       </c>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>0.93518888888888896</v>
+        <v>0.93555555555555558</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1703,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -1712,14 +1850,14 @@
         <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>0.91669999999999996</v>
+        <v>0.92</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="0"/>
-        <v>0.96296666666666653</v>
+        <v>0.9622222222222222</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1739,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1748,14 +1886,14 @@
         <v>1</v>
       </c>
       <c r="I8" s="3">
-        <v>0.95833333333333304</v>
+        <v>0.96</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="0"/>
-        <v>0.96759259259259245</v>
+        <v>0.96666666666666656</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1838,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>0.91666666666666696</v>
+        <v>0.92</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1847,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.54</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1863,7 +2001,7 @@
       </c>
       <c r="K11" s="6">
         <f t="shared" si="0"/>
-        <v>0.93981481481481488</v>
+        <v>0.94000000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>0.16669999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1892,14 +2030,14 @@
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="0"/>
-        <v>0.87963333333333327</v>
+        <v>0.87777777777777777</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1927,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>